<commit_message>
15.07.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/July/All Details/15.07.2020/MC Balance Transfer July 2020.xlsx
+++ b/2020/July/All Details/15.07.2020/MC Balance Transfer July 2020.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="114">
   <si>
     <t>Date</t>
   </si>
@@ -351,9 +351,6 @@
     <t xml:space="preserve">Naimul ZSM </t>
   </si>
   <si>
-    <t>S.A Mobile</t>
-  </si>
-  <si>
     <t>12.07.2020</t>
   </si>
   <si>
@@ -361,6 +358,12 @@
   </si>
   <si>
     <t>14.07.2020</t>
+  </si>
+  <si>
+    <t>15.07.20200</t>
+  </si>
+  <si>
+    <t>15.07.2020</t>
   </si>
 </sst>
 </file>
@@ -1180,7 +1183,7 @@
         <xdr:cNvPr id="1317" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1192,7 +1195,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1215,14 +1218,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -1532,7 +1535,7 @@
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="E94" sqref="E94"/>
+      <selection pane="bottomLeft" activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -2498,7 +2501,7 @@
     </row>
     <row r="14" spans="1:61" ht="12.6" customHeight="1">
       <c r="A14" s="14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B14" s="2">
         <v>285750</v>
@@ -2574,7 +2577,7 @@
     </row>
     <row r="15" spans="1:61" ht="12.6" customHeight="1">
       <c r="A15" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B15" s="2">
         <v>399690</v>
@@ -2650,7 +2653,7 @@
     </row>
     <row r="16" spans="1:61" ht="12.6" customHeight="1">
       <c r="A16" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B16" s="2">
         <v>335150</v>
@@ -2725,13 +2728,21 @@
       <c r="BI16" s="7"/>
     </row>
     <row r="17" spans="1:61" ht="12.6" customHeight="1">
-      <c r="A17" s="14"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+      <c r="A17" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="B17" s="2">
+        <v>548830</v>
+      </c>
+      <c r="C17" s="2">
+        <v>539000</v>
+      </c>
+      <c r="D17" s="2">
+        <v>490</v>
+      </c>
       <c r="E17" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>539490</v>
       </c>
       <c r="F17" s="95"/>
       <c r="G17" s="79"/>
@@ -3816,23 +3827,23 @@
       </c>
       <c r="B33" s="2">
         <f>SUM(B5:B32)</f>
-        <v>5528340</v>
+        <v>6077170</v>
       </c>
       <c r="C33" s="2">
         <f>SUM(C5:C32)</f>
-        <v>5991735</v>
+        <v>6530735</v>
       </c>
       <c r="D33" s="2">
         <f>SUM(D5:D32)</f>
-        <v>12715</v>
+        <v>13205</v>
       </c>
       <c r="E33" s="2">
         <f>SUM(E5:E32)</f>
-        <v>6004450</v>
+        <v>6543940</v>
       </c>
       <c r="F33" s="67">
         <f>B33-E33</f>
-        <v>-476110</v>
+        <v>-466770</v>
       </c>
       <c r="G33" s="81"/>
       <c r="H33" s="86"/>
@@ -4106,7 +4117,7 @@
         <v>5000</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E37" s="6"/>
       <c r="F37" s="95"/>
@@ -4319,7 +4330,7 @@
         <v>8500</v>
       </c>
       <c r="D40" s="122" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="95"/>
@@ -5496,10 +5507,10 @@
       </c>
       <c r="B58" s="30"/>
       <c r="C58" s="71">
-        <v>90000</v>
+        <v>98000</v>
       </c>
       <c r="D58" s="70" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="E58" s="3"/>
       <c r="F58" s="49"/>
@@ -5849,10 +5860,10 @@
       </c>
       <c r="B63" s="70"/>
       <c r="C63" s="134">
-        <v>170550</v>
+        <v>168770</v>
       </c>
       <c r="D63" s="70" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="E63" s="3"/>
       <c r="F63" s="48"/>
@@ -5934,7 +5945,7 @@
         <v>370070</v>
       </c>
       <c r="D64" s="72" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E64" s="3"/>
       <c r="F64" s="50"/>
@@ -6013,10 +6024,10 @@
       </c>
       <c r="B65" s="30"/>
       <c r="C65" s="71">
-        <v>190800</v>
+        <v>190410</v>
       </c>
       <c r="D65" s="70" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E65" s="3"/>
       <c r="F65" s="48"/>
@@ -6090,16 +6101,10 @@
       <c r="BI65" s="7"/>
     </row>
     <row r="66" spans="1:61" ht="12.75" customHeight="1">
-      <c r="A66" s="73" t="s">
-        <v>109</v>
-      </c>
+      <c r="A66" s="73"/>
       <c r="B66" s="70"/>
-      <c r="C66" s="71">
-        <v>2000</v>
-      </c>
-      <c r="D66" s="72" t="s">
-        <v>107</v>
-      </c>
+      <c r="C66" s="71"/>
+      <c r="D66" s="72"/>
       <c r="E66" s="3"/>
       <c r="F66" s="110"/>
       <c r="G66" s="13" t="s">
@@ -6420,10 +6425,16 @@
       <c r="BI69" s="7"/>
     </row>
     <row r="70" spans="1:61" ht="12.75" customHeight="1">
-      <c r="A70" s="73"/>
+      <c r="A70" s="73" t="s">
+        <v>57</v>
+      </c>
       <c r="B70" s="30"/>
-      <c r="C70" s="71"/>
-      <c r="D70" s="76"/>
+      <c r="C70" s="71">
+        <v>5510</v>
+      </c>
+      <c r="D70" s="76" t="s">
+        <v>113</v>
+      </c>
       <c r="E70" s="3"/>
       <c r="F70" s="110"/>
       <c r="G70" s="13" t="s">
@@ -8580,7 +8591,7 @@
       <c r="B98" s="145"/>
       <c r="C98" s="32">
         <f>SUM(C37:C97)</f>
-        <v>1596553</v>
+        <v>1605893</v>
       </c>
       <c r="D98" s="28"/>
       <c r="F98" s="110"/>
@@ -8735,7 +8746,7 @@
       <c r="B100" s="143"/>
       <c r="C100" s="29">
         <f>C98+L121</f>
-        <v>1596553</v>
+        <v>1605893</v>
       </c>
       <c r="D100" s="21"/>
       <c r="F100" s="48"/>

</xml_diff>